<commit_message>
Master add the answer in lession1
</commit_message>
<xml_diff>
--- a/Documentation/02_Task/Lession1.xlsx
+++ b/Documentation/02_Task/Lession1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>What is msp stand for?</t>
   </si>
@@ -26,6 +26,21 @@
   </si>
   <si>
     <t xml:space="preserve">Port printf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question </t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>This file defines all initialization functions to configure the IP instances according to the user configuration ( pin allocation, enabling of lock, use of DMA and interupt)</t>
+  </si>
+  <si>
+    <t>"stm32f7xx_hal_msp.c" (MSP -&gt;MCU Support Package ), t</t>
   </si>
 </sst>
 </file>
@@ -61,8 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,48 +385,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>